<commit_message>
Completed user spreadsheet imports.
</commit_message>
<xml_diff>
--- a/public/spreadsheets/users.xlsx
+++ b/public/spreadsheets/users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -40,6 +40,27 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">business_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ward</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ali</t>
   </si>
   <si>
@@ -52,6 +73,18 @@
     <t xml:space="preserve">amwinyi</t>
   </si>
   <si>
+    <t xml:space="preserve">Hub-agrodealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kigoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kigoma Mjini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gungu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Athumani</t>
   </si>
   <si>
@@ -64,6 +97,9 @@
     <t xml:space="preserve">anonga</t>
   </si>
   <si>
+    <t xml:space="preserve">Agrodealer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adam</t>
   </si>
   <si>
@@ -97,6 +133,9 @@
     <t xml:space="preserve">mwaziri</t>
   </si>
   <si>
+    <t xml:space="preserve">Reseller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amina</t>
   </si>
   <si>
@@ -109,6 +148,15 @@
     <t xml:space="preserve">amollel</t>
   </si>
   <si>
+    <t xml:space="preserve">Kagera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bukoba Mjini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kashai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wema</t>
   </si>
   <si>
@@ -119,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">wsepetu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitendaguro</t>
   </si>
 </sst>
 </file>
@@ -216,17 +267,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,145 +310,320 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>755437887</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">C2&amp;" Traders"</f>
+        <v>Mwinyi Traders</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>-4.869005</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>29.648337</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>754012345</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">C3&amp;" Traders"</f>
+        <v>Nonga Traders</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>-4.872377</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>29.649013</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>755437888</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="str">
+        <f aca="false">C4&amp;" Traders"</f>
+        <v>Daudi Traders</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>-4.873781</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>29.649221</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>755437889</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">C5&amp;" Traders"</f>
+        <v>Bundi Traders</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>-4.874001</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>29.649601</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>755437880</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">C6&amp;" Traders"</f>
+        <v>Waziri Traders</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>-4.875001</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>29.649941</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>754098098</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">C7&amp;" Traders"</f>
+        <v>Mollel Traders</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>-1.330705</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>31.809021</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>765434343</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>48</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <f aca="false">C8&amp;" Traders"</f>
+        <v>Sepetu Traders</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>-1.353445</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>31.797271</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>